<commit_message>
Iterador e nó duplo.
</commit_message>
<xml_diff>
--- a/Projeto02/MemóriaAlunoCurso-v2.xlsx
+++ b/Projeto02/MemóriaAlunoCurso-v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="45">
   <si>
     <t>null</t>
   </si>
@@ -132,6 +132,33 @@
   </si>
   <si>
     <t>caso 3</t>
+  </si>
+  <si>
+    <t>caso 6</t>
+  </si>
+  <si>
+    <t>lista duplamente encadeada</t>
+  </si>
+  <si>
+    <t>nó</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+  <si>
+    <t>exemplo</t>
+  </si>
+  <si>
+    <t>lista</t>
+  </si>
+  <si>
+    <t>duplamente</t>
+  </si>
+  <si>
+    <t>encadeada</t>
+  </si>
+  <si>
+    <t>iterator</t>
   </si>
 </sst>
 </file>
@@ -247,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -280,6 +307,13 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2564,106 +2598,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>41548</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>100054</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>386828</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>194071</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="71" name="Conector de Seta Reta 70"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5539772" y="5736226"/>
-          <a:ext cx="345280" cy="672086"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>395452</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>73779</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>521492</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>165538</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="72" name="Conector de Seta Reta 71"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8948245" y="5709951"/>
-          <a:ext cx="126040" cy="669828"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>13138</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>118241</xdr:rowOff>
@@ -3819,8 +3753,8 @@
       <xdr:rowOff>83344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>39414</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>85397</xdr:rowOff>
     </xdr:to>
@@ -3831,8 +3765,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1721890" y="15369327"/>
-          <a:ext cx="6870317" cy="2053"/>
+          <a:off x="1721890" y="19422378"/>
+          <a:ext cx="3802610" cy="2053"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4183,6 +4117,1106 @@
         <a:xfrm flipH="1">
           <a:off x="8803728" y="15451728"/>
           <a:ext cx="126040" cy="669828"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>453258</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>597775</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>137957</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Conector de Seta Reta 80"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4118741" y="23293552"/>
+          <a:ext cx="755431" cy="426991"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>512378</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>65690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>584638</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>118247</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Conector de Seta Reta 81"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1734206" y="23451207"/>
+          <a:ext cx="683173" cy="52557"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>183930</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>183932</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Conector de Seta Reta 115"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2627585" y="15391087"/>
+          <a:ext cx="6569" cy="656897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>164224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>111674</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="118" name="Conector de Seta Reta 117"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3672052" y="16619483"/>
+          <a:ext cx="604346" cy="335019"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419674</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>67209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>513694</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>132693</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="119" name="Conector de Seta Reta 118"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2863329" y="14190485"/>
+          <a:ext cx="94020" cy="636984"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>507945</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>84658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>597776</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>91966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="120" name="Conector de Seta Reta 119"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1729773" y="23667244"/>
+          <a:ext cx="700744" cy="7308"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>537834</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>92580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>68563</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>99149</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="128" name="Conector de Seta Reta 127"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4814231" y="28700425"/>
+          <a:ext cx="752556" cy="400707"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>558362</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>124810</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="129" name="Conector de Seta Reta 128"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2391103" y="29251604"/>
+          <a:ext cx="788276" cy="223344"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466396</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>98534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604344</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>105102</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="130" name="Conector de Seta Reta 129"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6575534" y="2233448"/>
+          <a:ext cx="748862" cy="400706"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>466396</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>98534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>604344</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>105102</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="131" name="Conector de Seta Reta 130"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9019189" y="2233448"/>
+          <a:ext cx="748862" cy="400706"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>374430</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>91965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>170793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="132" name="Conector de Seta Reta 131"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4039913" y="29691724"/>
+          <a:ext cx="6569" cy="656897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>402020</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>67004</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>408589</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>145832</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="133" name="Conector de Seta Reta 132"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8954813" y="29666763"/>
+          <a:ext cx="6569" cy="656897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>396766</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>88024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403335</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>166852</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="134" name="Conector de Seta Reta 133"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6505904" y="29687783"/>
+          <a:ext cx="6569" cy="656897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>545224</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>124811</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="135" name="Conector de Seta Reta 134"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1767052" y="2187466"/>
+          <a:ext cx="801414" cy="32844"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>532086</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>118241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>59122</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>85397</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="136" name="Conector de Seta Reta 135"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1753914" y="26788241"/>
+          <a:ext cx="748863" cy="361294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>499734</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>126739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>30463</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>133308</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="138" name="Conector de Seta Reta 137"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4165217" y="26796739"/>
+          <a:ext cx="752556" cy="400707"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>137948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223345</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>19707</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="143" name="Conector de Seta Reta 142"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3271345" y="27202086"/>
+          <a:ext cx="6569" cy="656897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>132696</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>112987</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="144" name="Conector de Seta Reta 143"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2469931" y="29593190"/>
+          <a:ext cx="717334" cy="112987"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>587266</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>153714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114302</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>120870</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="145" name="Conector de Seta Reta 144"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4863663" y="29359335"/>
+          <a:ext cx="748863" cy="361294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>529459</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>155028</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>56495</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>122184</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="Conector de Seta Reta 145"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7249511" y="29360649"/>
+          <a:ext cx="748863" cy="361294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>507945</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>84658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>131379</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="147" name="Conector de Seta Reta 146"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2340686" y="29677848"/>
+          <a:ext cx="5627469" cy="46721"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>545224</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85396</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91965</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="148" name="Conector de Seta Reta 147"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1156138" y="2594741"/>
+          <a:ext cx="6260224" cy="807983"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4477,10 +5511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S108"/>
+  <dimension ref="A2:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4491,21 +5525,21 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="M4" s="7" t="s">
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="M4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -4588,21 +5622,21 @@
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="I11" s="7" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="I11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="M11" s="7" t="s">
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="M11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -4661,21 +5695,30 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="7" t="s">
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="I17" s="7" t="s">
+      <c r="F17" s="12"/>
+      <c r="I17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="M17" s="7" t="s">
+      <c r="J17" s="12"/>
+      <c r="M17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="4"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="I18" s="2"/>
@@ -4764,11 +5807,11 @@
         <v>19</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
@@ -4838,14 +5881,14 @@
       <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="H32" s="7" t="s">
+      <c r="F32" s="12"/>
+      <c r="H32" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E33" s="2"/>
@@ -4930,11 +5973,11 @@
         <v>19</v>
       </c>
       <c r="C49" s="6"/>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
@@ -5009,14 +6052,14 @@
       <c r="A55" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="H55" s="7" t="s">
+      <c r="F55" s="12"/>
+      <c r="H55" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E56" s="2"/>
@@ -5121,11 +6164,11 @@
         <v>19</v>
       </c>
       <c r="C77" s="6"/>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
     </row>
     <row r="78" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
@@ -5202,14 +6245,14 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E83" s="7" t="s">
+      <c r="E83" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F83" s="7"/>
-      <c r="H83" s="7" t="s">
+      <c r="F83" s="12"/>
+      <c r="H83" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="7"/>
+      <c r="I83" s="12"/>
     </row>
     <row r="84" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E84" s="2"/>
@@ -5277,11 +6320,11 @@
         <v>19</v>
       </c>
       <c r="C98" s="6"/>
-      <c r="E98" s="7" t="s">
+      <c r="E98" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="2"/>
@@ -5359,14 +6402,14 @@
       <c r="K103" s="11"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E104" s="7" t="s">
+      <c r="E104" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="7"/>
-      <c r="H104" s="7" t="s">
+      <c r="F104" s="12"/>
+      <c r="H104" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I104" s="7"/>
+      <c r="I104" s="12"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E105" s="2"/>
@@ -5421,8 +6464,388 @@
         <v>31</v>
       </c>
     </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="E116" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" s="7"/>
+      <c r="E120" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+    </row>
+    <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="I121" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="3"/>
+      <c r="C122" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="4"/>
+      <c r="C123" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E126" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F126" s="12"/>
+    </row>
+    <row r="127" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+    </row>
+    <row r="128" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E128" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E129" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D137" s="13"/>
+      <c r="E137" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+    </row>
+    <row r="138" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>37</v>
+      </c>
+      <c r="D138" s="13"/>
+      <c r="E138" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F138" s="14"/>
+      <c r="G138" s="14"/>
+      <c r="H138" s="13"/>
+    </row>
+    <row r="139" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D139" s="13"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="13"/>
+    </row>
+    <row r="140" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D140" s="13"/>
+      <c r="E140" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H140" s="13"/>
+    </row>
+    <row r="141" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D141" s="13"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="13"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+    </row>
+    <row r="144" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G144" s="14"/>
+      <c r="H144" s="13"/>
+    </row>
+    <row r="145" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="13"/>
+    </row>
+    <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H146" s="13"/>
+    </row>
+    <row r="147" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G147" s="4">
+        <v>9</v>
+      </c>
+      <c r="H147" s="13"/>
+    </row>
+    <row r="151" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D151" s="7"/>
+      <c r="F151" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G151" s="12"/>
+      <c r="H151" s="12"/>
+      <c r="J151" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K151" s="12"/>
+      <c r="L151" s="12"/>
+      <c r="N151" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O151" s="12"/>
+      <c r="P151" s="12"/>
+    </row>
+    <row r="152" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+      <c r="L152" s="2"/>
+      <c r="N152" s="2"/>
+      <c r="O152" s="2"/>
+      <c r="P152" s="2"/>
+      <c r="R152" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>41</v>
+      </c>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L153" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O153" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P153" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>42</v>
+      </c>
+      <c r="C154" s="4"/>
+      <c r="D154" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F157" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="12"/>
+      <c r="J157" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K157" s="12"/>
+      <c r="N157" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O157" s="12"/>
+    </row>
+    <row r="158" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="J158" s="2"/>
+      <c r="K158" s="2"/>
+      <c r="N158" s="2"/>
+      <c r="O158" s="2"/>
+    </row>
+    <row r="159" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F159" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K159" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N159" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O159" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F160" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G160" s="4">
+        <v>9</v>
+      </c>
+      <c r="J160" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K160" s="4">
+        <v>5</v>
+      </c>
+      <c r="N160" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O160" s="4">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="31">
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="J151:L151"/>
+    <mergeCell ref="N151:P151"/>
+    <mergeCell ref="F157:G157"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="N157:O157"/>
+    <mergeCell ref="E120:G120"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="E26:G26"/>
     <mergeCell ref="E98:G98"/>
     <mergeCell ref="E104:F104"/>
     <mergeCell ref="H104:I104"/>
@@ -5432,18 +6855,6 @@
     <mergeCell ref="E77:G77"/>
     <mergeCell ref="E83:F83"/>
     <mergeCell ref="H83:I83"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="M11:O11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisão sobre lista encadeada.
</commit_message>
<xml_diff>
--- a/Projeto02/MemóriaAlunoCurso-v2.xlsx
+++ b/Projeto02/MemóriaAlunoCurso-v2.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="47">
   <si>
     <t>null</t>
   </si>
@@ -160,6 +161,12 @@
   <si>
     <t>iterator</t>
   </si>
+  <si>
+    <t>encadeamento simples</t>
+  </si>
+  <si>
+    <t>duplamente encadeada</t>
+  </si>
 </sst>
 </file>
 
@@ -274,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -307,11 +314,19 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -336,13 +351,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>545224</xdr:colOff>
+      <xdr:colOff>545225</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>52552</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>124810</xdr:colOff>
+      <xdr:rowOff>65690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>597776</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>85396</xdr:rowOff>
     </xdr:to>
@@ -353,8 +368,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4920155" y="1018190"/>
-          <a:ext cx="801414" cy="32844"/>
+          <a:off x="1767053" y="834259"/>
+          <a:ext cx="663464" cy="19706"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -985,16 +1000,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>7882</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>564931</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>53865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>145831</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>60433</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105103</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1003,8 +1018,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4284279" y="1019503"/>
-          <a:ext cx="748862" cy="400706"/>
+          <a:off x="4230414" y="1019503"/>
+          <a:ext cx="802727" cy="248307"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4997,16 +5012,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>26276</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>518949</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>112988</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>132696</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>112987</xdr:rowOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5014,9 +5029,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2469931" y="29593190"/>
-          <a:ext cx="717334" cy="112987"/>
+        <a:xfrm flipH="1">
+          <a:off x="2351690" y="29712747"/>
+          <a:ext cx="835575" cy="530770"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5200,23 +5215,528 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>545224</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>65689</xdr:rowOff>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>578069</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="148" name="Conector de Seta Reta 147"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1156138" y="2607879"/>
+          <a:ext cx="1254672" cy="794846"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>545224</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector de Seta Reta 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1764424" y="1240971"/>
+          <a:ext cx="684862" cy="9196"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>550667</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85396</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector de Seta Reta 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6048891" y="1280948"/>
+          <a:ext cx="1282075" cy="354724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>559605</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604344</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>122422</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector de Seta Reta 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6668743" y="3185948"/>
+          <a:ext cx="1266567" cy="424595"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>550667</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector de Seta Reta 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4208267" y="1447800"/>
+          <a:ext cx="657647" cy="205139"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>604157</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92529</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector de Seta Reta 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2432957" y="3614057"/>
+          <a:ext cx="647700" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>168729</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector de Seta Reta 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5475514" y="3646715"/>
+          <a:ext cx="1257300" cy="48985"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>144517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector de Seta Reta 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3626069" y="3238500"/>
+          <a:ext cx="656897" cy="293165"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>588767</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>91965</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="148" name="Conector de Seta Reta 147"/>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74509</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector de Seta Reta 26"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1156138" y="2594741"/>
-          <a:ext cx="6260224" cy="807983"/>
+          <a:off x="588767" y="3396343"/>
+          <a:ext cx="641319" cy="3752"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>91966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>94405</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32844</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector de Seta Reta 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="827690" y="3580087"/>
+          <a:ext cx="488543" cy="328447"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>497856</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>137948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>584638</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector de Seta Reta 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10272477" y="3231931"/>
+          <a:ext cx="697695" cy="356277"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5513,8 +6033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G14"/>
+    <sheetView topLeftCell="B130" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144:G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5525,21 +6045,21 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="I4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="M4" s="12" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="M4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -5613,6 +6133,11 @@
       </c>
       <c r="O7" s="4"/>
     </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>19</v>
@@ -5622,21 +6147,21 @@
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="I11" s="12" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="I11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="M11" s="12" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="M11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -5704,18 +6229,18 @@
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="I17" s="12" t="s">
+      <c r="F17" s="14"/>
+      <c r="I17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="M17" s="12" t="s">
+      <c r="J17" s="14"/>
+      <c r="M17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="12"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
@@ -5807,11 +6332,11 @@
         <v>19</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
@@ -5881,14 +6406,14 @@
       <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="H32" s="12" t="s">
+      <c r="F32" s="14"/>
+      <c r="H32" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="12"/>
+      <c r="I32" s="14"/>
     </row>
     <row r="33" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E33" s="2"/>
@@ -5973,11 +6498,11 @@
         <v>19</v>
       </c>
       <c r="C49" s="6"/>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
@@ -6052,14 +6577,14 @@
       <c r="A55" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="12"/>
-      <c r="H55" s="12" t="s">
+      <c r="F55" s="14"/>
+      <c r="H55" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="12"/>
+      <c r="I55" s="14"/>
     </row>
     <row r="56" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E56" s="2"/>
@@ -6164,11 +6689,11 @@
         <v>19</v>
       </c>
       <c r="C77" s="6"/>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
@@ -6245,14 +6770,14 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E83" s="12" t="s">
+      <c r="E83" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F83" s="12"/>
-      <c r="H83" s="12" t="s">
+      <c r="F83" s="14"/>
+      <c r="H83" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="12"/>
+      <c r="I83" s="14"/>
     </row>
     <row r="84" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E84" s="2"/>
@@ -6320,11 +6845,11 @@
         <v>19</v>
       </c>
       <c r="C98" s="6"/>
-      <c r="E98" s="12" t="s">
+      <c r="E98" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="2"/>
@@ -6402,14 +6927,14 @@
       <c r="K103" s="11"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E104" s="12" t="s">
+      <c r="E104" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="12"/>
-      <c r="H104" s="12" t="s">
+      <c r="F104" s="14"/>
+      <c r="H104" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I104" s="12"/>
+      <c r="I104" s="14"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E105" s="2"/>
@@ -6482,11 +7007,11 @@
         <v>19</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="E120" s="12" t="s">
+      <c r="E120" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
     </row>
     <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="2"/>
@@ -6531,10 +7056,10 @@
       </c>
     </row>
     <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E126" s="12" t="s">
+      <c r="E126" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F126" s="12"/>
+      <c r="F126" s="14"/>
     </row>
     <row r="127" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E127" s="2"/>
@@ -6562,35 +7087,35 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D137" s="13"/>
-      <c r="E137" s="13" t="s">
+      <c r="D137" s="12"/>
+      <c r="E137" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="13"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
     </row>
     <row r="138" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>37</v>
       </c>
-      <c r="D138" s="13"/>
-      <c r="E138" s="14" t="s">
+      <c r="D138" s="12"/>
+      <c r="E138" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="13"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="15"/>
+      <c r="H138" s="12"/>
     </row>
     <row r="139" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D139" s="13"/>
+      <c r="D139" s="12"/>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="13"/>
+      <c r="H139" s="12"/>
     </row>
     <row r="140" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D140" s="13"/>
+      <c r="D140" s="12"/>
       <c r="E140" s="3" t="s">
         <v>39</v>
       </c>
@@ -6600,87 +7125,87 @@
       <c r="G140" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H140" s="13"/>
+      <c r="H140" s="12"/>
     </row>
     <row r="141" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D141" s="13"/>
+      <c r="D141" s="12"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
       <c r="G141" s="4"/>
-      <c r="H141" s="13"/>
+      <c r="H141" s="12"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
+      <c r="F142" s="12"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="12"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D143" s="13"/>
-      <c r="E143" s="13"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="13"/>
-      <c r="H143" s="13"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
+      <c r="G143" s="12"/>
+      <c r="H143" s="12"/>
     </row>
     <row r="144" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
-      <c r="F144" s="14" t="s">
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
+      <c r="F144" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G144" s="14"/>
-      <c r="H144" s="13"/>
+      <c r="G144" s="15"/>
+      <c r="H144" s="12"/>
     </row>
     <row r="145" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D145" s="13"/>
-      <c r="E145" s="13"/>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-      <c r="H145" s="13"/>
+      <c r="H145" s="12"/>
     </row>
     <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D146" s="13"/>
-      <c r="E146" s="13"/>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
       <c r="F146" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H146" s="13"/>
+      <c r="H146" s="12"/>
     </row>
     <row r="147" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
       <c r="F147" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G147" s="4">
         <v>9</v>
       </c>
-      <c r="H147" s="13"/>
+      <c r="H147" s="12"/>
     </row>
     <row r="151" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C151" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D151" s="7"/>
-      <c r="F151" s="12" t="s">
+      <c r="F151" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G151" s="12"/>
-      <c r="H151" s="12"/>
-      <c r="J151" s="12" t="s">
+      <c r="G151" s="14"/>
+      <c r="H151" s="14"/>
+      <c r="J151" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K151" s="12"/>
-      <c r="L151" s="12"/>
-      <c r="N151" s="12" t="s">
+      <c r="K151" s="14"/>
+      <c r="L151" s="14"/>
+      <c r="N151" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O151" s="12"/>
-      <c r="P151" s="12"/>
+      <c r="O151" s="14"/>
+      <c r="P151" s="14"/>
     </row>
     <row r="152" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
@@ -6761,18 +7286,21 @@
       </c>
     </row>
     <row r="157" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F157" s="12" t="s">
+      <c r="D157" t="s">
+        <v>0</v>
+      </c>
+      <c r="F157" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G157" s="12"/>
-      <c r="J157" s="12" t="s">
+      <c r="G157" s="14"/>
+      <c r="J157" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K157" s="12"/>
-      <c r="N157" s="12" t="s">
+      <c r="K157" s="14"/>
+      <c r="N157" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O157" s="12"/>
+      <c r="O157" s="14"/>
     </row>
     <row r="158" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F158" s="2"/>
@@ -6836,6 +7364,15 @@
     <mergeCell ref="E138:G138"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="I4:K4"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="H83:I83"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
@@ -6846,15 +7383,294 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="H83:I83"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:S31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="H6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="M6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>9</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="4">
+        <v>7</v>
+      </c>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G15" s="12"/>
+      <c r="H15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="18"/>
+      <c r="N16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="12"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="N18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="4">
+        <v>7</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="12"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="M6:O6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>